<commit_message>
Minor changes to Printerautomation.py.
</commit_message>
<xml_diff>
--- a/TestData/Staple.xlsx
+++ b/TestData/Staple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F33DC-B41A-4B1A-82F5-7631788A8060}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC1DEDC-CF33-4CDD-A782-6A6E7A7F2C65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="3840" windowWidth="21600" windowHeight="11505" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>